<commit_message>
Ajout de la mise à jour d'un projet
</commit_message>
<xml_diff>
--- a/vpp/echeancier.xlsx
+++ b/vpp/echeancier.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\le_hu\Desktop\_maville25\maville25\vpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A26CD402-E5EE-4391-8287-105EEC3BDD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFE3D17-1ADE-485E-9763-4F1A58C089F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C7E56CDF-29BD-4D8B-9EC8-831F4455B1AF}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -529,7 +529,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -542,48 +541,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -925,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE594CC1-F2EF-4ED5-8F74-FED4CCE2C94E}">
-  <dimension ref="C1:X15"/>
+  <dimension ref="C1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="S11" sqref="S11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -942,96 +939,96 @@
     <col min="22" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:24" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="3:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="40" t="s">
+    <row r="1" spans="3:23" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="3:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="29">
+      <c r="D2" s="43"/>
+      <c r="E2" s="28">
         <v>1</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="29">
         <v>2</v>
       </c>
-      <c r="G2" s="30">
+      <c r="G2" s="29">
         <v>3</v>
       </c>
-      <c r="H2" s="30">
+      <c r="H2" s="29">
         <v>4</v>
       </c>
-      <c r="I2" s="30">
+      <c r="I2" s="29">
         <v>5</v>
       </c>
-      <c r="J2" s="30">
+      <c r="J2" s="29">
         <v>6</v>
       </c>
-      <c r="K2" s="30">
+      <c r="K2" s="29">
         <v>7</v>
       </c>
-      <c r="L2" s="30">
+      <c r="L2" s="29">
         <v>8</v>
       </c>
-      <c r="M2" s="30">
+      <c r="M2" s="29">
         <v>9</v>
       </c>
-      <c r="N2" s="30">
+      <c r="N2" s="29">
         <v>10</v>
       </c>
-      <c r="O2" s="30">
+      <c r="O2" s="29">
         <v>11</v>
       </c>
-      <c r="P2" s="30">
+      <c r="P2" s="29">
         <v>12</v>
       </c>
-      <c r="Q2" s="30">
+      <c r="Q2" s="29">
         <v>13</v>
       </c>
-      <c r="R2" s="42">
+      <c r="R2" s="33">
         <v>14</v>
       </c>
-      <c r="S2" s="42">
+      <c r="S2" s="33">
         <v>15</v>
       </c>
-      <c r="T2" s="31" t="s">
+      <c r="T2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="32"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="41"/>
     </row>
-    <row r="3" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="43" t="s">
+    <row r="3" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="27"/>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27"/>
-      <c r="T3" s="28" t="s">
+      <c r="D3" s="45"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="24"/>
+      <c r="U3" s="22"/>
+      <c r="V3" s="22"/>
+      <c r="W3" s="23"/>
     </row>
-    <row r="4" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="44" t="s">
+    <row r="4" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="35"/>
       <c r="E4" s="4"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
@@ -1054,11 +1051,11 @@
       <c r="V4" s="12"/>
       <c r="W4" s="13"/>
     </row>
-    <row r="5" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="45" t="s">
+    <row r="5" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
       <c r="G5" s="3"/>
@@ -1081,18 +1078,18 @@
       <c r="V5" s="10"/>
       <c r="W5" s="11"/>
     </row>
-    <row r="6" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="44" t="s">
+    <row r="6" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="36"/>
+      <c r="D6" s="35"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="3"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="33"/>
+      <c r="K6" s="3"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -1108,18 +1105,18 @@
       <c r="V6" s="12"/>
       <c r="W6" s="13"/>
     </row>
-    <row r="7" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="45" t="s">
+    <row r="7" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="37"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="8"/>
       <c r="F7" s="15"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="3"/>
       <c r="J7" s="16"/>
-      <c r="K7" s="33"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -1135,18 +1132,18 @@
       <c r="V7" s="10"/>
       <c r="W7" s="11"/>
     </row>
-    <row r="8" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="44" t="s">
+    <row r="8" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="36"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="33"/>
+      <c r="K8" s="3"/>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
@@ -1161,13 +1158,12 @@
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="13"/>
-      <c r="X8" s="22"/>
     </row>
-    <row r="9" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="45" t="s">
+    <row r="9" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="37"/>
+      <c r="D9" s="39"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="9"/>
@@ -1175,7 +1171,6 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="46"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1190,11 +1185,11 @@
       <c r="V9" s="10"/>
       <c r="W9" s="11"/>
     </row>
-    <row r="10" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="44" t="s">
+    <row r="10" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="36"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="4"/>
       <c r="F10" s="3"/>
       <c r="G10" s="5"/>
@@ -1217,11 +1212,11 @@
       <c r="V10" s="12"/>
       <c r="W10" s="13"/>
     </row>
-    <row r="11" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="45" t="s">
+    <row r="11" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="37"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="4"/>
       <c r="F11" s="3"/>
       <c r="G11" s="9"/>
@@ -1234,9 +1229,9 @@
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
       <c r="P11" s="9"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
       <c r="T11" s="17" t="s">
         <v>8</v>
       </c>
@@ -1244,11 +1239,11 @@
       <c r="V11" s="10"/>
       <c r="W11" s="11"/>
     </row>
-    <row r="12" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="44" t="s">
+    <row r="12" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="36"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="4"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -1271,11 +1266,11 @@
       <c r="V12" s="12"/>
       <c r="W12" s="13"/>
     </row>
-    <row r="13" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="45" t="s">
+    <row r="13" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="37"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1284,10 +1279,10 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
@@ -1298,11 +1293,11 @@
       <c r="V13" s="10"/>
       <c r="W13" s="11"/>
     </row>
-    <row r="14" spans="3:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="44" t="s">
+    <row r="14" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="4"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -1311,13 +1306,13 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="38"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="31"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
       <c r="T14" s="18" t="s">
         <v>10</v>
       </c>
@@ -1325,11 +1320,11 @@
       <c r="V14" s="12"/>
       <c r="W14" s="13"/>
     </row>
-    <row r="15" spans="3:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="47" t="s">
+    <row r="15" spans="3:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="48"/>
+      <c r="D15" s="37"/>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1341,7 +1336,7 @@
       <c r="M15" s="7"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
-      <c r="P15" s="34"/>
+      <c r="P15" s="30"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
@@ -1354,6 +1349,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C8:D8"/>
@@ -1362,13 +1364,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mise à jour de l'échancier
</commit_message>
<xml_diff>
--- a/vpp/echeancier.xlsx
+++ b/vpp/echeancier.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\le_hu\Desktop\_maville25\maville25\vpp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFE3D17-1ADE-485E-9763-4F1A58C089F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3F7181-D6B9-42F3-90B4-3EEF07D14EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C7E56CDF-29BD-4D8B-9EC8-831F4455B1AF}"/>
   </bookViews>
@@ -553,34 +553,34 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -925,7 +925,7 @@
   <dimension ref="C1:W15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -941,10 +941,10 @@
   <sheetData>
     <row r="1" spans="3:23" s="2" customFormat="1" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="3:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="43"/>
+      <c r="D2" s="41"/>
       <c r="E2" s="28">
         <v>1</v>
       </c>
@@ -990,18 +990,18 @@
       <c r="S2" s="33">
         <v>15</v>
       </c>
-      <c r="T2" s="40" t="s">
+      <c r="T2" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="41"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="39"/>
     </row>
     <row r="3" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="45"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="24"/>
       <c r="F3" s="25"/>
       <c r="G3" s="26"/>
@@ -1052,10 +1052,10 @@
       <c r="W4" s="13"/>
     </row>
     <row r="5" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="39"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="8"/>
       <c r="F5" s="9"/>
       <c r="G5" s="3"/>
@@ -1106,10 +1106,10 @@
       <c r="W6" s="13"/>
     </row>
     <row r="7" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="39"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="8"/>
       <c r="F7" s="15"/>
       <c r="G7" s="9"/>
@@ -1160,10 +1160,10 @@
       <c r="W8" s="13"/>
     </row>
     <row r="9" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="39"/>
+      <c r="D9" s="37"/>
       <c r="E9" s="4"/>
       <c r="F9" s="3"/>
       <c r="G9" s="9"/>
@@ -1213,10 +1213,10 @@
       <c r="W10" s="13"/>
     </row>
     <row r="11" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="39"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="4"/>
       <c r="F11" s="3"/>
       <c r="G11" s="9"/>
@@ -1267,10 +1267,10 @@
       <c r="W12" s="13"/>
     </row>
     <row r="13" spans="3:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="39"/>
+      <c r="D13" s="37"/>
       <c r="E13" s="4"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1285,7 +1285,7 @@
       <c r="P13" s="32"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
+      <c r="S13" s="32"/>
       <c r="T13" s="17" t="s">
         <v>19</v>
       </c>
@@ -1321,10 +1321,10 @@
       <c r="W14" s="13"/>
     </row>
     <row r="15" spans="3:23" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="37"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1349,13 +1349,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="T2:W2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C8:D8"/>
@@ -1364,6 +1357,13 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="T2:W2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>